<commit_message>
Support returning raw Jave objects when parsing an Excel sheet
</commit_message>
<xml_diff>
--- a/site/sample/excel/test.xlsx
+++ b/site/sample/excel/test.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgoeschl/work/github/sgoeschl/freemarker-cli/site/sample/office/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgoeschl/work/github/sgoeschl/freemarker-cli/site/sample/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271A5A9C-0022-B84B-B8DB-4CDA65EB7BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -59,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0.00"/>
@@ -149,6 +156,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -416,11 +426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <v>42736</v>
+        <v>42766</v>
       </c>
       <c r="C2" s="6">
         <v>100</v>
@@ -486,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="5">
-        <v>42737</v>
+        <v>42794</v>
       </c>
       <c r="C3" s="6">
         <v>200</v>

</xml_diff>